<commit_message>
modify automatic code logic
</commit_message>
<xml_diff>
--- a/Source/Extend/Driver/gpio/Template/gpio_config.xlsx
+++ b/Source/Extend/Driver/gpio/Template/gpio_config.xlsx
@@ -3,12 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE7AC2E9-D73E-4EED-B5D1-619E8185564B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B5D16C12-3936-4FAB-9831-6DCF58CBC37F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GPIO" sheetId="1" r:id="rId1"/>
+    <sheet name="include" sheetId="2" r:id="rId1"/>
+    <sheet name="define" sheetId="3" r:id="rId2"/>
+    <sheet name="variable" sheetId="4" r:id="rId3"/>
+    <sheet name="function" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,45 +23,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
   <si>
     <t>GPIOA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIOx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PINx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpio.h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN11</t>
+  </si>
+  <si>
+    <t>PIN12</t>
+  </si>
+  <si>
+    <t>PIN13</t>
+  </si>
+  <si>
+    <t>PIN0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN1</t>
+  </si>
+  <si>
+    <t>PIN2</t>
+  </si>
+  <si>
+    <t>PIN3</t>
+  </si>
+  <si>
+    <t>PIN4</t>
+  </si>
+  <si>
+    <t>PIN5</t>
+  </si>
+  <si>
+    <t>PIN6</t>
+  </si>
+  <si>
+    <t>PIN7</t>
+  </si>
+  <si>
+    <t>PIN8</t>
+  </si>
+  <si>
+    <t>PIN9</t>
+  </si>
+  <si>
     <t>PIN10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PULL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OUT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GPIOx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PINx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IN/OUT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PULL/DROP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SET/RESET</t>
+  </si>
+  <si>
+    <t>IN_OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PULL_DROP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SET_RESET</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -383,30 +429,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC2AA58-F644-468F-AF5A-DE3A59A8BEE1}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3A9FA8-FFFC-4BB3-BFE5-C006EDD1D07D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC667F59-9696-40B5-B63C-14CAB0899A37}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -414,16 +515,237 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>